<commit_message>
listas de engenharia sendo feitas
</commit_message>
<xml_diff>
--- a/4 - IES300A Engenharia de Software III/Exercícios - Lista N1/CasosDeUsoTextuais.xlsx
+++ b/4 - IES300A Engenharia de Software III/Exercícios - Lista N1/CasosDeUsoTextuais.xlsx
@@ -8,7 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan2" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CSU01" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="CSU05" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="26">
   <si>
     <t xml:space="preserve">Caso de Uso: 05</t>
   </si>
@@ -130,13 +131,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,35 +152,168 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF172B4D"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFBDD7EE"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFBDD7EE"/>
-        <bgColor rgb="FF99CCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -191,7 +324,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -215,58 +348,126 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="35" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="36" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -291,7 +492,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -320,14 +521,198 @@
   </sheetPr>
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B40" activeCellId="0" sqref="B40"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="136.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="82.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Arial,Regular"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,Regular"&amp;10Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="103.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.53"/>
   </cols>
   <sheetData>
@@ -486,6 +871,7 @@
       </c>
       <c r="B21" s="3"/>
     </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>